<commit_message>
Update - Version 0.61
- preping
</commit_message>
<xml_diff>
--- a/PCU GUI Idea/Excel Templates/Excel Data/test123.xlsx
+++ b/PCU GUI Idea/Excel Templates/Excel Data/test123.xlsx
@@ -185,7 +185,9 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView zoomScale="100" topLeftCell="A1" workbookViewId="0" showGridLines="true" showRowColHeaders="true" view="normal"/>
+    <sheetView zoomScale="100" topLeftCell="A1" workbookViewId="0" showGridLines="true" showRowColHeaders="true" view="normal">
+      <selection activeCell="R24" sqref="R24:R24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="false" defaultColWidth="9.28125" defaultRowHeight="15"/>
   <sheetData>

</xml_diff>